<commit_message>
fixed incorrect average height formula
</commit_message>
<xml_diff>
--- a/data/end_montage_table.xlsx
+++ b/data/end_montage_table.xlsx
@@ -573,16 +573,16 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>2.723758260825445</v>
+        <v>2.730995758697492</v>
       </c>
       <c r="G3" t="n">
-        <v>1.710422563765221</v>
+        <v>1.722369395643906</v>
       </c>
       <c r="H3" t="n">
-        <v>2.868511180811435</v>
+        <v>2.878921494922184</v>
       </c>
       <c r="I3" t="n">
-        <v>1.849892545914591</v>
+        <v>1.859543089110336</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -610,46 +610,46 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>61.154</v>
+        <v>65.292</v>
       </c>
       <c r="C4" t="n">
-        <v>57.145</v>
+        <v>60.727</v>
       </c>
       <c r="D4" t="n">
-        <v>53.666</v>
+        <v>56.775</v>
       </c>
       <c r="E4" t="n">
-        <v>52.1</v>
+        <v>55</v>
       </c>
       <c r="F4" t="n">
-        <v>110.688</v>
+        <v>114.321</v>
       </c>
       <c r="G4" t="n">
-        <v>78.46899999999999</v>
+        <v>82.09</v>
       </c>
       <c r="H4" t="n">
-        <v>114.946</v>
+        <v>118.689</v>
       </c>
       <c r="I4" t="n">
-        <v>83.205</v>
+        <v>86.77800000000001</v>
       </c>
       <c r="J4" t="n">
-        <v>50.636</v>
+        <v>53.345</v>
       </c>
       <c r="K4" t="n">
-        <v>47.983</v>
+        <v>50.355</v>
       </c>
       <c r="L4" t="n">
-        <v>45.646</v>
+        <v>47.736</v>
       </c>
       <c r="M4" t="n">
-        <v>41.731</v>
+        <v>43.382</v>
       </c>
       <c r="N4" t="n">
-        <v>38.587</v>
+        <v>39.921</v>
       </c>
       <c r="O4" t="n">
-        <v>36.007</v>
+        <v>37.108</v>
       </c>
     </row>
     <row r="5">
@@ -659,46 +659,46 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>30.002</v>
+        <v>32.032</v>
       </c>
       <c r="C5" t="n">
-        <v>28.035</v>
+        <v>29.793</v>
       </c>
       <c r="D5" t="n">
-        <v>26.329</v>
+        <v>27.854</v>
       </c>
       <c r="E5" t="n">
-        <v>25.56</v>
+        <v>26.983</v>
       </c>
       <c r="F5" t="n">
-        <v>54.304</v>
+        <v>56.086</v>
       </c>
       <c r="G5" t="n">
-        <v>38.497</v>
+        <v>40.273</v>
       </c>
       <c r="H5" t="n">
-        <v>56.393</v>
+        <v>58.229</v>
       </c>
       <c r="I5" t="n">
-        <v>40.82</v>
+        <v>42.573</v>
       </c>
       <c r="J5" t="n">
-        <v>24.842</v>
+        <v>26.171</v>
       </c>
       <c r="K5" t="n">
-        <v>23.54</v>
+        <v>24.704</v>
       </c>
       <c r="L5" t="n">
-        <v>22.394</v>
+        <v>23.419</v>
       </c>
       <c r="M5" t="n">
-        <v>20.473</v>
+        <v>21.283</v>
       </c>
       <c r="N5" t="n">
-        <v>18.931</v>
+        <v>19.585</v>
       </c>
       <c r="O5" t="n">
-        <v>17.665</v>
+        <v>18.205</v>
       </c>
     </row>
     <row r="6">
@@ -708,46 +708,46 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1863.991</v>
+        <v>1990.118</v>
       </c>
       <c r="C6" t="n">
-        <v>1741.795</v>
+        <v>1850.976</v>
       </c>
       <c r="D6" t="n">
-        <v>1635.755</v>
+        <v>1730.518</v>
       </c>
       <c r="E6" t="n">
-        <v>1588.022</v>
+        <v>1676.415</v>
       </c>
       <c r="F6" t="n">
-        <v>1238.656</v>
+        <v>1275.921</v>
       </c>
       <c r="G6" t="n">
-        <v>1398.343</v>
+        <v>1452.723</v>
       </c>
       <c r="H6" t="n">
-        <v>1221.395</v>
+        <v>1256.607</v>
       </c>
       <c r="I6" t="n">
-        <v>1370.951</v>
+        <v>1422.402</v>
       </c>
       <c r="J6" t="n">
-        <v>1543.399</v>
+        <v>1625.97</v>
       </c>
       <c r="K6" t="n">
-        <v>1462.535</v>
+        <v>1534.834</v>
       </c>
       <c r="L6" t="n">
-        <v>1391.303</v>
+        <v>1455.006</v>
       </c>
       <c r="M6" t="n">
-        <v>1271.972</v>
+        <v>1322.295</v>
       </c>
       <c r="N6" t="n">
-        <v>1176.142</v>
+        <v>1216.803</v>
       </c>
       <c r="O6" t="n">
-        <v>1097.503</v>
+        <v>1131.062</v>
       </c>
     </row>
     <row r="7">
@@ -757,46 +757,46 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>22.458</v>
+        <v>26.642</v>
       </c>
       <c r="C7" t="n">
-        <v>20.986</v>
+        <v>24.78</v>
       </c>
       <c r="D7" t="n">
-        <v>19.709</v>
+        <v>23.167</v>
       </c>
       <c r="E7" t="n">
-        <v>19.133</v>
+        <v>22.443</v>
       </c>
       <c r="F7" t="n">
-        <v>40.65</v>
+        <v>46.649</v>
       </c>
       <c r="G7" t="n">
-        <v>28.817</v>
+        <v>33.497</v>
       </c>
       <c r="H7" t="n">
-        <v>42.213</v>
+        <v>48.431</v>
       </c>
       <c r="I7" t="n">
-        <v>30.556</v>
+        <v>35.41</v>
       </c>
       <c r="J7" t="n">
-        <v>18.596</v>
+        <v>21.767</v>
       </c>
       <c r="K7" t="n">
-        <v>17.621</v>
+        <v>20.547</v>
       </c>
       <c r="L7" t="n">
-        <v>16.763</v>
+        <v>19.478</v>
       </c>
       <c r="M7" t="n">
-        <v>15.325</v>
+        <v>17.702</v>
       </c>
       <c r="N7" t="n">
-        <v>14.171</v>
+        <v>16.29</v>
       </c>
       <c r="O7" t="n">
-        <v>13.223</v>
+        <v>15.142</v>
       </c>
     </row>
     <row r="8">
@@ -806,46 +806,46 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.142</v>
+        <v>4.816</v>
       </c>
       <c r="C8" t="n">
-        <v>5.503</v>
+        <v>5.178</v>
       </c>
       <c r="D8" t="n">
-        <v>5.86</v>
+        <v>5.539</v>
       </c>
       <c r="E8" t="n">
-        <v>6.037</v>
+        <v>5.718</v>
       </c>
       <c r="F8" t="n">
-        <v>7.742</v>
+        <v>7.516</v>
       </c>
       <c r="G8" t="n">
-        <v>6.857</v>
+        <v>6.6</v>
       </c>
       <c r="H8" t="n">
-        <v>7.852</v>
+        <v>7.631</v>
       </c>
       <c r="I8" t="n">
-        <v>6.994</v>
+        <v>6.74</v>
       </c>
       <c r="J8" t="n">
-        <v>6.211</v>
+        <v>5.896</v>
       </c>
       <c r="K8" t="n">
-        <v>6.555</v>
+        <v>6.246</v>
       </c>
       <c r="L8" t="n">
-        <v>6.891</v>
+        <v>6.589</v>
       </c>
       <c r="M8" t="n">
-        <v>7.539</v>
+        <v>7.252</v>
       </c>
       <c r="N8" t="n">
-        <v>8.154999999999999</v>
+        <v>7.882</v>
       </c>
       <c r="O8" t="n">
-        <v>8.74</v>
+        <v>8.48</v>
       </c>
     </row>
     <row r="9">
@@ -855,46 +855,46 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>7.1</v>
+        <v>6.65</v>
       </c>
       <c r="C9" t="n">
-        <v>7.599</v>
+        <v>7.15</v>
       </c>
       <c r="D9" t="n">
-        <v>8.093</v>
+        <v>7.649</v>
       </c>
       <c r="E9" t="n">
-        <v>8.336</v>
+        <v>7.896</v>
       </c>
       <c r="F9" t="n">
-        <v>10.694</v>
+        <v>10.38</v>
       </c>
       <c r="G9" t="n">
-        <v>9.468999999999999</v>
+        <v>9.114000000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>10.845</v>
+        <v>10.54</v>
       </c>
       <c r="I9" t="n">
-        <v>9.659000000000001</v>
+        <v>9.308999999999999</v>
       </c>
       <c r="J9" t="n">
-        <v>8.577999999999999</v>
+        <v>8.141</v>
       </c>
       <c r="K9" t="n">
-        <v>9.053000000000001</v>
+        <v>8.625999999999999</v>
       </c>
       <c r="L9" t="n">
-        <v>9.516999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="M9" t="n">
-        <v>10.413</v>
+        <v>10.015</v>
       </c>
       <c r="N9" t="n">
-        <v>11.264</v>
+        <v>10.886</v>
       </c>
       <c r="O9" t="n">
-        <v>12.074</v>
+        <v>11.714</v>
       </c>
     </row>
     <row r="10">
@@ -904,46 +904,46 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.546</v>
+        <v>4.258</v>
       </c>
       <c r="C10" t="n">
-        <v>4.866</v>
+        <v>4.578</v>
       </c>
       <c r="D10" t="n">
-        <v>5.181</v>
+        <v>4.897</v>
       </c>
       <c r="E10" t="n">
-        <v>5.337</v>
+        <v>5.056</v>
       </c>
       <c r="F10" t="n">
-        <v>6.845</v>
+        <v>6.645</v>
       </c>
       <c r="G10" t="n">
-        <v>6.062</v>
+        <v>5.835</v>
       </c>
       <c r="H10" t="n">
-        <v>6.942</v>
+        <v>6.747</v>
       </c>
       <c r="I10" t="n">
-        <v>6.183</v>
+        <v>5.96</v>
       </c>
       <c r="J10" t="n">
-        <v>5.492</v>
+        <v>5.213</v>
       </c>
       <c r="K10" t="n">
-        <v>5.796</v>
+        <v>5.522</v>
       </c>
       <c r="L10" t="n">
-        <v>6.093</v>
+        <v>5.826</v>
       </c>
       <c r="M10" t="n">
-        <v>6.665</v>
+        <v>6.411</v>
       </c>
       <c r="N10" t="n">
-        <v>7.21</v>
+        <v>6.968</v>
       </c>
       <c r="O10" t="n">
-        <v>7.727</v>
+        <v>7.498</v>
       </c>
     </row>
     <row r="11">
@@ -953,46 +953,46 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6.039</v>
+        <v>5.656</v>
       </c>
       <c r="C11" t="n">
-        <v>6.463</v>
+        <v>6.081</v>
       </c>
       <c r="D11" t="n">
-        <v>6.883</v>
+        <v>6.505</v>
       </c>
       <c r="E11" t="n">
-        <v>7.09</v>
+        <v>6.715</v>
       </c>
       <c r="F11" t="n">
-        <v>9.093999999999999</v>
+        <v>8.827</v>
       </c>
       <c r="G11" t="n">
-        <v>8.053000000000001</v>
+        <v>7.751</v>
       </c>
       <c r="H11" t="n">
-        <v>9.223000000000001</v>
+        <v>8.962999999999999</v>
       </c>
       <c r="I11" t="n">
-        <v>8.214</v>
+        <v>7.917</v>
       </c>
       <c r="J11" t="n">
-        <v>7.295</v>
+        <v>6.924</v>
       </c>
       <c r="K11" t="n">
-        <v>7.699</v>
+        <v>7.336</v>
       </c>
       <c r="L11" t="n">
-        <v>8.093999999999999</v>
+        <v>7.739</v>
       </c>
       <c r="M11" t="n">
-        <v>8.855</v>
+        <v>8.516999999999999</v>
       </c>
       <c r="N11" t="n">
-        <v>9.577999999999999</v>
+        <v>9.257</v>
       </c>
       <c r="O11" t="n">
-        <v>10.267</v>
+        <v>9.961</v>
       </c>
     </row>
     <row r="12">
@@ -1002,46 +1002,46 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.322</v>
+        <v>1.238</v>
       </c>
       <c r="C12" t="n">
-        <v>1.415</v>
+        <v>1.332</v>
       </c>
       <c r="D12" t="n">
-        <v>1.507</v>
+        <v>1.424</v>
       </c>
       <c r="E12" t="n">
-        <v>1.552</v>
+        <v>1.47</v>
       </c>
       <c r="F12" t="n">
-        <v>1.99</v>
+        <v>1.932</v>
       </c>
       <c r="G12" t="n">
-        <v>1.763</v>
+        <v>1.697</v>
       </c>
       <c r="H12" t="n">
-        <v>2.018</v>
+        <v>1.962</v>
       </c>
       <c r="I12" t="n">
-        <v>1.798</v>
+        <v>1.733</v>
       </c>
       <c r="J12" t="n">
-        <v>1.597</v>
+        <v>1.516</v>
       </c>
       <c r="K12" t="n">
-        <v>1.685</v>
+        <v>1.606</v>
       </c>
       <c r="L12" t="n">
-        <v>1.772</v>
+        <v>1.694</v>
       </c>
       <c r="M12" t="n">
-        <v>1.938</v>
+        <v>1.864</v>
       </c>
       <c r="N12" t="n">
-        <v>2.096</v>
+        <v>2.026</v>
       </c>
       <c r="O12" t="n">
-        <v>2.246</v>
+        <v>2.179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>